<commit_message>
added split docs in to sentances function into topic model plus, added ICS_utils, refactored trend analysis functions, updated ICS journal notebook, added tests
</commit_message>
<xml_diff>
--- a/results/ICS_bertopic_combined_topics_Jun-23-2022/hazard_interpretation_v1.xlsx
+++ b/results/ICS_bertopic_combined_topics_Jun-23-2022/hazard_interpretation_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\results\ICS_bertopic_combined_topics_Jun-23-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7CB114-5EAF-412D-ACC8-440B771DD273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A52FD6-1FFB-49C8-BFD7-FB4F4DF04520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2964" yWindow="2964" windowWidth="16464" windowHeight="9300" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>Hazard level 1 topics</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Hazard Noun/Subject</t>
   </si>
   <si>
-    <t>lifted</t>
-  </si>
-  <si>
     <t>Evacuations</t>
   </si>
   <si>
@@ -145,54 +142,30 @@
     <t>Injury</t>
   </si>
   <si>
-    <t>branch</t>
-  </si>
-  <si>
     <t>low wind, lower wind, favorable</t>
   </si>
   <si>
-    <t>lawson, carson, leonard</t>
-  </si>
-  <si>
     <t>violation, law, possible law, law violation, possible law violation</t>
   </si>
   <si>
-    <t>type, type team, transition, transition type, type organization, command,  ic, transfer, type ic, transition type organization, transfer command, imt, type imt, type, command, transition, imt2, transfer, team, transfer command, imt3, assumed, local, type, transition, command, organization, transfer,  ic, transfer command, type team, type organization, transition type, type ic, transitioned, ict4, local type, command type, imt</t>
-  </si>
-  <si>
     <t>lightning, thunderstorms, lightning, thunderstorm, thunderstorms area, afternoon thunderstorms, afternoon thunderstorms started, thunderstorms next, thunderstorms started, thunderstorms started several, winds associated thunderstorms, thunderstorms fuels, thunderstorms fuels extremely</t>
   </si>
   <si>
-    <t>smoke, smoke impacts, smoke impacts local, smoke impact, potential smoke, smokes, concern, air quality</t>
-  </si>
-  <si>
     <t>open, reopen, lifted</t>
   </si>
   <si>
     <t>wind, erratic, winds, mph, red flag, warning, red flag warning, flag warning, winds, red flag warnings, flag warnings, warnings, red flag conditions, winds low, winds, gusty, winds low, wind, erratic, gusty winds, winds low rh, mph, strong, erratic winds, winds winds, rh winds, winds low rhs</t>
   </si>
   <si>
-    <t xml:space="preserve">rh, dry, red flag, warning, red flag warning, flag warning, low, red flag warnings, flag warnings, warnings, red flag conditions, flag conditions, drought, dry, low, low humidity, drought conditions, dry fuels, dry conditions, hot, prolonged drought, prolonged, fuel, low fuel, drying, dry weather, moistures, low rh, low rhs, </t>
-  </si>
-  <si>
-    <t>evacuation, evacuation, evacuations, evacuated, homes evacuated, order, mandatory, evacuation order</t>
-  </si>
-  <si>
     <t>5, 13, 20, 25, 32, 50, 63</t>
   </si>
   <si>
     <t>3, 6, 8, 21, 69</t>
   </si>
   <si>
-    <t>terrain, steep, difficult, steep terrain, limited, terrain, steep, access, steep terrain, difficult, terrain steep, rugged, access steep, limited, access steep terrain, limited access, inaccessible, terrain limited access, terrain difficult, inaccessible terrain, terrain limited, rugged terrain, difficult access, steep rugged, steep inaccessible terrain, snag, snags, rollouts, canyon, side canyon, inaccessible terrain extremely, terrain extremely dry, terrain extremely, treacherous</t>
-  </si>
-  <si>
     <t>18, 41, 46, 60, 62, 68, 73, 86, 88</t>
   </si>
   <si>
-    <t>okefenokee, habitat, sage grouse, sage, grouse, grouse habitat, sage grouse habitat, critical sage grouse, critical sage, critical, juniper, national forest, habitat, endangered species habitat, threatened, species, endangered, species habitat, endangered species, critical habitat, critical, sensitive, tortoise, sparrow, seaside sparrow, seaside, sensitive resource critical, resource critical habitat, protection sensitive resource, protection sensitive, threatened endangered, pyramid lake, pyramid, spread snail, prevention spread snail, spread snail pyramid, snail pyramid, prevention spread, snail, snail pyramid lake, habitat protection heritage, species habitat protection, protection heritage, protection heritage resources, mist threatenedendangered, mist threatenedendangered species, beaches, soil, organic, organic soil</t>
-  </si>
-  <si>
     <t>5, 6, 8, 12, 15, 18, 22, 26, 31, 33, 42, 43, 50, 63, 76, 79, 82, 87, 89</t>
   </si>
   <si>
@@ -202,9 +175,6 @@
     <t>1, 20, 88, 97</t>
   </si>
   <si>
-    <t xml:space="preserve"> rain, received, precipitation, recieved, inches, rainfall, inches rain, received rain, light, received precipitation, significant, inch, rain today, area received, rain received, light rain, precip</t>
-  </si>
-  <si>
     <t>11, 26, 29, 82, 97</t>
   </si>
   <si>
@@ -214,21 +184,9 @@
     <t>24, 41, 101</t>
   </si>
   <si>
-    <t>ranch, goat, sheep, cattle, grazing, grazing, cattle, loss, forage grazing permittees, loss forage grazing, forage grazing, grazing permittees, loss forage, ranches threat resource, ranches threat, cattle association ranches, association ranches threat, association ranches, cattle association, ranch</t>
-  </si>
-  <si>
-    <t>17, 28, 100, 102, 105</t>
-  </si>
-  <si>
     <t>40, 48, 108</t>
   </si>
   <si>
-    <t>military, base, unexploded ordinance area, ordinance area, military, unexploded, ordinance, unexploded ordinance, special use, military training, located special, located special use, special use training, training site, use training site</t>
-  </si>
-  <si>
-    <t>mapping, acreage, accurate, accurate mapping, due accurate, due accurate mapping, acreage due, gps, increase, better mapping, due better</t>
-  </si>
-  <si>
     <t>4, 15, 29, 38, 63, 42, 92</t>
   </si>
   <si>
@@ -238,35 +196,95 @@
     <t>27, 29, 36, 80, 88, 15, 26</t>
   </si>
   <si>
-    <t>30, 42, 35</t>
-  </si>
-  <si>
-    <t>injury, hospital, firefighter, injuries, transported, treated, medical, heat, released, minor, reported, ankle, burns, injury reported, injured, transported hospital, treated released, degree, degree burns, eye, elbow</t>
-  </si>
-  <si>
-    <t>36, 43, 73, 89, 94, 95, 90</t>
-  </si>
-  <si>
-    <t>tribal commercial timberland, private tribal commercial, cultural, extremely yurok karuk, extremely yurok, yurok karuk, yurok karuk tolowa, karuk tolowa, karuk tolowa cultural, tolowa, tolowa cultural concerns, tolowa cultural, yurok, cultural concerns, heritage, tribal, cultural, national archeological, potential impact national, impact national archeological, national archeological sites, impact national, sites potential impact, archeological sites potential, archeological, resource site, cultural resource site, archeological sites, access cultural, access cultural resource, hikers, national monument, tribe, community</t>
-  </si>
-  <si>
-    <t>lack, critical, support, critical resource need, resource need, unstaffed, logistical concerns, shortage</t>
-  </si>
-  <si>
-    <t>infrastructure, utility, facilities infrastructure, power, pipeline, gas, powerlines, gas pipeline, large 250kv, large 250kv power, 250kv power serves, power serves, 250kv power, large gas, serves large, large gas pipeline, serves large gas, power serves large, 250kv,, gas pipeline potential, pipeline potential, water spout, water, telephone</t>
-  </si>
-  <si>
     <t>36, 59, 39, 88, 37</t>
   </si>
   <si>
-    <t>closure, highway, closed, traffic, closures, road closure, road closures, hwy, roads,  rd, road closed, lanes</t>
+    <t>ranch, goat, sheep, cattle, grazing, grazing, cattle, forage grazing permittees, loss forage grazing, forage grazing, grazing permittees, loss forage, ranches threat resource, ranches threat, cattle association ranches, association ranches threat, association ranches, cattle association, ranch</t>
+  </si>
+  <si>
+    <t>accurate mapping, due accurate, due accurate mapping, acreage due, gps, better mapping, due better</t>
+  </si>
+  <si>
+    <t>infrastructure, utility, facilities infrastructure, power, pipeline, gas, powerlines, gas pipeline, large 250kv, large 250kv power, 250kv power serves, power serves, 250kv power, large gas, serves large, large gas pipeline, serves large gas, power serves large, 250kv,, gas pipeline potential, pipeline potential, telephone, watershed</t>
+  </si>
+  <si>
+    <t>17, 28, 100, 102, 105, 48, 42, 58</t>
+  </si>
+  <si>
+    <t>30, 42, 35, 48, 91</t>
+  </si>
+  <si>
+    <t>15, 5, 6, 17, 39, 42, 84, 102</t>
+  </si>
+  <si>
+    <t>air operations, grounded, aircraft grounded</t>
+  </si>
+  <si>
+    <t>Aerial Grounding</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rain , precipitation, received rain, inches, rainfall, inches rain, received rain, received precipitation,  inch, rain today, area received, rain received, light rain, precip</t>
+  </si>
+  <si>
+    <t>evacuation, evacuation, evacuations, evacuated, homes evacuated, mandatory, evacuation order</t>
+  </si>
+  <si>
+    <t>okefenokee, habitat, sage grouse, grouse, grouse habitat, sage grouse habitat, critical sage grouse, critical sage, juniper, national forest, habitat, endangered species habitat, species, endangered, species habitat, endangered species, critical habitat, tortoise, sparrow, seaside sparrow, seaside, sensitive resource critical, resource critical habitat, protection sensitive resource, protection sensitive, threatened endangered, pyramid lake, spread snail, prevention spread snail, spread snail pyramid, snail pyramid, prevention spread, snail, snail pyramid lake, habitat protection heritage, species habitat protection, protection heritage, protection heritage resources, mist threatenedendangered, mist threatenedendangered species, beaches, soil, organic, organic soil</t>
+  </si>
+  <si>
+    <t>terrain, steep, difficult terraub, steep terrain, limited access, terrain, steep, steep terrain, terrain steep, rugged, access steep, access steep terrain, limited access, inaccessible, terrain limited access, terrain difficult, inaccessible terrain, terrain limited, rugged terrain, difficult access, steep rugged, steep inaccessible terrain, snag, snags, rollouts, canyon, side canyon, inaccessible terrain extremely, terrain extremely dry, terrain extremely, treacherous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lack, critical resource, critical resource need, resource need, unstaffed, logistical concerns, shortage, resources are needed, shared, competition</t>
+  </si>
+  <si>
+    <t>smoke, smoke impacts, smoke impacts local, smoke impact, potential smoke, air quality</t>
+  </si>
+  <si>
+    <t>type team, command transition, transition type, type organization, transfer, type ic, transition type organization, transfer command, type imt, imt2, transfer, transfer command, imt3, assumed, transition, command, transfer, transfer command, type team, type organization, transition type, type ic, transitioned, ict4, local type, command type</t>
+  </si>
+  <si>
+    <t>dry, red flag, red flag warning, flag warning, low relative humidity, red flag warnings, flag warnings, red flag conditions, flag conditions, drought, dry, low fuel, low humidity, drought conditions, dry fuels, dry conditions, hot, prolonged drought, prolonged, low fuel, drying, dry weather, moistures, low rh, low rhs, lower humidity</t>
+  </si>
+  <si>
+    <t>highway, closed, closures on, road closure, road closures, hwy, roads closed, road closed, lanes, closure on</t>
+  </si>
+  <si>
+    <t>branch, goat fire, goat creek</t>
+  </si>
+  <si>
+    <t>elbow pass, treated fuels</t>
+  </si>
+  <si>
+    <t>injury, hospital, injuries, transported, treated, medical, heat exhaustion, heat stroke, minor injur, ankle, injury reported, injured, transported hospital, treated released, degree, degree burns, eye, elbow</t>
+  </si>
+  <si>
+    <t>arson</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>36, 43, 73, 89, 94, 95, 90, 80</t>
+  </si>
+  <si>
+    <t>tribal commercial timberland, private tribal commercial, cultural, extremely yurok karuk, extremely yurok, yurok karuk, yurok karuk tolowa, karuk tolowa, karuk tolowa cultural, tolowa, tolowa cultural concerns, tolowa cultural, yurok, cultural concerns, heritage, tribal, cultural, national archeological, potential impact national, impact national archeological, national archeological sites, impact national, sites potential impact, archeological sites potential, archeological, resource site, cultural resource site, archeological sites, access cultural, access cultural resource, hikers, national monument, tribe, historic, recreation, campground, camp ground</t>
+  </si>
+  <si>
+    <t>added camp ground</t>
+  </si>
+  <si>
+    <t>lifted, lift</t>
+  </si>
+  <si>
+    <t>military, military base, unexploded ordinance area, ordinance area, military, unexploded, ordinance, unexploded ordinance, special use, military training, located special, located special use, special use training, training site, use training site,  fort , uxo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,6 +296,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -309,10 +333,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,15 +703,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -721,272 +747,295 @@
       <c r="R1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="T1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="P5" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="R5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>51</v>
-      </c>
-      <c r="P5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="R7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="P6" t="s">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P8" t="s">
         <v>31</v>
       </c>
-      <c r="R6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" t="s">
-        <v>32</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="R8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="P8" t="s">
-        <v>32</v>
-      </c>
-      <c r="R8" t="s">
+      <c r="E9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="P9" t="s">
-        <v>32</v>
-      </c>
-      <c r="R9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="N11" t="s">
         <v>38</v>
       </c>
-      <c r="P10" t="s">
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="2" t="s">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>67</v>
+      </c>
+      <c r="P12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" t="s">
+        <v>32</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" t="s">
+        <v>77</v>
+      </c>
+      <c r="P14" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
         <v>66</v>
       </c>
-      <c r="E11" t="s">
-        <v>74</v>
-      </c>
-      <c r="N11" t="s">
-        <v>43</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="P15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="P16" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P12" t="s">
-        <v>32</v>
-      </c>
-      <c r="R12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="P13" t="s">
-        <v>33</v>
-      </c>
-      <c r="R13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
-      </c>
-      <c r="P14" t="s">
-        <v>33</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" t="s">
-        <v>71</v>
-      </c>
-      <c r="P15" t="s">
-        <v>31</v>
-      </c>
-      <c r="R15" s="2" t="s">
+      <c r="R16" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
-        <v>41</v>
-      </c>
-      <c r="P16" t="s">
-        <v>32</v>
-      </c>
-      <c r="R16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="P17" t="s">
-        <v>33</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="N18" t="s">
+        <v>72</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="N19" t="s">
+        <v>71</v>
+      </c>
+      <c r="P19" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>59</v>
       </c>
-      <c r="N19" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" t="s">
-        <v>33</v>
-      </c>
-      <c r="R19" s="2" t="s">
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20" t="s">
         <v>30</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>